<commit_message>
Do delete all related study results and registration results when user want to re-import study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_K3_CNTT.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_K3_CNTT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\StudyProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F98EEE-7796-4C21-A70D-2CD87BF695E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D7B61-D4EB-4636-BEA6-CB913AF1C434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1212,6 +1212,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>413658</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>32889</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>26429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1E2762-ECA7-3F70-F7EE-152E38E3F29B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18571029" y="903513"/>
+          <a:ext cx="2667231" cy="3520745"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="190500" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="70000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1598,9 +1657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5718,6 +5777,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>